<commit_message>
Update DRAM Data for analysis
</commit_message>
<xml_diff>
--- a/DRAM_System_Analysis/Data/subarray_analysis_trace_summary.xlsx
+++ b/DRAM_System_Analysis/Data/subarray_analysis_trace_summary.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gota\Desktop\DRAM_Analyze\Master_Thesis_MC\DRAM_System_Analysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B516296F-5CAD-47FD-8E50-DBCFEDBF4AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AB0B5E-6D18-4669-BE2F-14EBBE1E8170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{C6FCE36D-0945-43F2-8BD5-F027151F16D3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{C6FCE36D-0945-43F2-8BD5-F027151F16D3}"/>
   </bookViews>
   <sheets>
     <sheet name="subarray_analysis_trace_summary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1305,7 +1318,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>98.710090600000001</c:v>
+                  <c:v>92.032623299999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1417,7 +1430,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>98.7346103</c:v>
+                  <c:v>64.4584045</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2054,7 +2067,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>95.617370600000001</c:v>
+                  <c:v>95.616889999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2166,7 +2179,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>96.844512899999998</c:v>
+                  <c:v>90.213058500000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2278,7 +2291,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>96.8646241</c:v>
+                  <c:v>63.107902500000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2930,7 +2943,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1472.56323446838</c:v>
+                  <c:v>1472.55877376282</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3031,7 +3044,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1816.6537871466999</c:v>
+                  <c:v>1821.6952828809699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3132,7 +3145,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2513.0808323671499</c:v>
+                  <c:v>2549.56629034462</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3769,7 +3782,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1466.1738805413102</c:v>
+                  <c:v>1466.1741363893002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3881,7 +3894,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1810.4794685331699</c:v>
+                  <c:v>1814.8394300054199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3993,7 +4006,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2506.9269444568099</c:v>
+                  <c:v>2538.6137428965999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4145,6 +4158,518 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1672027551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>subarray_analysis_trace_summary!$H$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No Refresh 32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>subarray_analysis_trace_summary!$I$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bandwidth</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>subarray_analysis_trace_summary!$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>86.7328033</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BD51-4145-A2BE-9524D00BBF26}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>subarray_analysis_trace_summary!$H$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No Refresh 64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>subarray_analysis_trace_summary!$I$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bandwidth</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>subarray_analysis_trace_summary!$I$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>95.334396400000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BD51-4145-A2BE-9524D00BBF26}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>subarray_analysis_trace_summary!$H$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No Refresh 128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>subarray_analysis_trace_summary!$I$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bandwidth</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>subarray_analysis_trace_summary!$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>99.942398100000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BD51-4145-A2BE-9524D00BBF26}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>subarray_analysis_trace_summary!$H$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No Refresh 256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>subarray_analysis_trace_summary!$I$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bandwidth</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>subarray_analysis_trace_summary!$I$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>94.335998500000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-BD51-4145-A2BE-9524D00BBF26}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>subarray_analysis_trace_summary!$H$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No Refresh 512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>subarray_analysis_trace_summary!$I$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bandwidth</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>subarray_analysis_trace_summary!$I$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>65.664001499999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-BD51-4145-A2BE-9524D00BBF26}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="92675872"/>
+        <c:axId val="92671072"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="92675872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="92671072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="92671072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="92675872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4384,6 +4909,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5894,6 +6459,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6516,8 +7584,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>446941</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>8282</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6537,6 +7605,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>766142</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>156541</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>37272</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>828</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="圖表 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F73E1D5-F22C-73F8-2EFF-DF58CD45F795}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6864,8 +7968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679830D5-6DBA-432D-A016-457AE55A7427}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -7363,6 +8467,9 @@
       <c r="H24" t="s">
         <v>24</v>
       </c>
+      <c r="I24">
+        <v>86.7328033</v>
+      </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25">
@@ -7380,13 +8487,16 @@
       <c r="H25" t="s">
         <v>25</v>
       </c>
+      <c r="I25">
+        <v>95.334396400000003</v>
+      </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>128</v>
       </c>
       <c r="C26">
-        <v>95.617370600000001</v>
+        <v>95.616889999999998</v>
       </c>
       <c r="E26">
         <v>128</v>
@@ -7396,6 +8506,9 @@
       </c>
       <c r="H26" t="s">
         <v>26</v>
+      </c>
+      <c r="I26">
+        <v>99.942398100000005</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
@@ -7403,16 +8516,19 @@
         <v>256</v>
       </c>
       <c r="C27">
-        <v>96.844512899999998</v>
+        <v>90.213058500000002</v>
       </c>
       <c r="E27">
         <v>256</v>
       </c>
       <c r="F27">
-        <v>98.710090600000001</v>
+        <v>92.032623299999997</v>
       </c>
       <c r="H27" t="s">
         <v>27</v>
+      </c>
+      <c r="I27">
+        <v>94.335998500000002</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
@@ -7420,16 +8536,19 @@
         <v>512</v>
       </c>
       <c r="C28">
-        <v>96.8646241</v>
+        <v>63.107902500000002</v>
       </c>
       <c r="E28">
         <v>512</v>
       </c>
       <c r="F28">
-        <v>98.7346103</v>
+        <v>64.4584045</v>
       </c>
       <c r="H28" t="s">
         <v>28</v>
+      </c>
+      <c r="I28">
+        <v>65.664001499999998</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
@@ -7498,24 +8617,24 @@
         <v>128</v>
       </c>
       <c r="C33">
-        <v>1472563234.46838</v>
+        <v>1472558773.76282</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
-        <v>1472.56323446838</v>
+        <v>1472.55877376282</v>
       </c>
       <c r="E33">
         <v>128</v>
       </c>
       <c r="F33">
-        <v>1466173880.5413101</v>
+        <v>1466174136.3893001</v>
       </c>
       <c r="G33">
         <v>128</v>
       </c>
       <c r="H33">
         <f>F33/1000000</f>
-        <v>1466.1738805413102</v>
+        <v>1466.1741363893002</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -7523,24 +8642,24 @@
         <v>256</v>
       </c>
       <c r="C34">
-        <v>1816653787.1466999</v>
+        <v>1821695282.88097</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>1816.6537871466999</v>
+        <v>1821.6952828809699</v>
       </c>
       <c r="E34">
         <v>256</v>
       </c>
       <c r="F34">
-        <v>1810479468.53317</v>
+        <v>1814839430.00542</v>
       </c>
       <c r="G34">
         <v>256</v>
       </c>
       <c r="H34">
         <f>F34/1000000</f>
-        <v>1810.4794685331699</v>
+        <v>1814.8394300054199</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -7548,24 +8667,24 @@
         <v>512</v>
       </c>
       <c r="C35">
-        <v>2513080832.3671498</v>
+        <v>2549566290.3446202</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
-        <v>2513.0808323671499</v>
+        <v>2549.56629034462</v>
       </c>
       <c r="E35">
         <v>512</v>
       </c>
       <c r="F35">
-        <v>2506926944.45681</v>
+        <v>2538613742.8965998</v>
       </c>
       <c r="G35">
         <v>512</v>
       </c>
       <c r="H35">
         <f>F35/1000000</f>
-        <v>2506.9269444568099</v>
+        <v>2538.6137428965999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>